<commit_message>
Complete job summary py file
</commit_message>
<xml_diff>
--- a/database/Templates/JobSumTemplate.xlsx
+++ b/database/Templates/JobSumTemplate.xlsx
@@ -8,35 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kurtm\Documents\GitHub\PerformanceHub\database\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{41880536-4722-4B0B-A326-6239068E43F2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4DC25BB1-9DA9-493F-B925-A1B7A486FF31}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8685" tabRatio="820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PRINTOUT" sheetId="14" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="15" r:id="rId2"/>
-    <sheet name="Areas Summary" sheetId="9" r:id="rId3"/>
-    <sheet name="Areas Summary (By Material)" sheetId="10" r:id="rId4"/>
-    <sheet name="Spool Location" sheetId="7" r:id="rId5"/>
-    <sheet name="Shorts by Scope" sheetId="1" r:id="rId6"/>
-    <sheet name="Purchased by Scope" sheetId="11" r:id="rId7"/>
-    <sheet name="No Material by Scope" sheetId="12" r:id="rId8"/>
-    <sheet name="Spool Missing Valve Only" sheetId="13" r:id="rId9"/>
-    <sheet name="List of Shorts" sheetId="2" r:id="rId10"/>
-    <sheet name="Spools by Scope" sheetId="4" r:id="rId11"/>
-    <sheet name="List of Spools" sheetId="8" r:id="rId12"/>
-    <sheet name="Discrepancies" sheetId="6" r:id="rId13"/>
+    <sheet name="Areas Summary" sheetId="9" r:id="rId2"/>
+    <sheet name="Areas Summary (By Material)" sheetId="10" r:id="rId3"/>
+    <sheet name="Spool Location" sheetId="7" r:id="rId4"/>
+    <sheet name="Shorts by Scope" sheetId="1" r:id="rId5"/>
+    <sheet name="Purchased by Scope" sheetId="11" r:id="rId6"/>
+    <sheet name="No Material by Scope" sheetId="12" r:id="rId7"/>
+    <sheet name="Spool Missing Valve Only" sheetId="13" r:id="rId8"/>
+    <sheet name="Spools by Scope" sheetId="4" r:id="rId9"/>
+    <sheet name="Discrepancies" sheetId="6" r:id="rId10"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'List of Shorts'!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11">'List of Spools'!$A$1:$Z$1</definedName>
-  </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="45">
   <si>
     <t>Performance</t>
   </si>
@@ -65,39 +58,6 @@
     <t>Supports</t>
   </si>
   <si>
-    <t>Missing Valves</t>
-  </si>
-  <si>
-    <t>Material</t>
-  </si>
-  <si>
-    <t>Spool</t>
-  </si>
-  <si>
-    <t>Scope</t>
-  </si>
-  <si>
-    <t>Tag #</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Multiplier</t>
-  </si>
-  <si>
-    <t>Missing Flanges</t>
-  </si>
-  <si>
-    <t>Missing Fittings</t>
-  </si>
-  <si>
-    <t>Missing Supports</t>
-  </si>
-  <si>
     <t>Issued</t>
   </si>
   <si>
@@ -105,18 +65,6 @@
   </si>
   <si>
     <t>Workable</t>
-  </si>
-  <si>
-    <t>Total Items</t>
-  </si>
-  <si>
-    <t>Missing Pipe</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Priorty</t>
   </si>
   <si>
     <t>ITEMS</t>
@@ -137,12 +85,6 @@
     <t>Area</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
-    <t>Dormant</t>
-  </si>
-  <si>
     <t>Priority</t>
   </si>
   <si>
@@ -158,12 +100,6 @@
     <t>Delivered</t>
   </si>
   <si>
-    <t>Lifespan</t>
-  </si>
-  <si>
-    <t>Hold Item</t>
-  </si>
-  <si>
     <t>Not Workable</t>
   </si>
   <si>
@@ -177,12 +113,6 @@
   </si>
   <si>
     <t>Not on Line List</t>
-  </si>
-  <si>
-    <t>Total Pipe</t>
-  </si>
-  <si>
-    <t>Missing Items (Ea.)</t>
   </si>
   <si>
     <t>TOTAL SHORTS (ITEM QUANTITIES)</t>
@@ -222,9 +152,6 @@
   </si>
   <si>
     <t>Delivered %</t>
-  </si>
-  <si>
-    <t>Shop</t>
   </si>
   <si>
     <t>PM In Status Report (Not in Line List)</t>
@@ -708,16 +635,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -750,9 +674,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -788,18 +709,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -8271,13 +8180,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -8594,10 +8503,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N101"/>
+  <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8611,346 +8520,349 @@
     <col min="14" max="14" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="52" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="55"/>
+    <row r="1" spans="1:12" s="46" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="55"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="49"/>
     </row>
-    <row r="2" spans="1:12" s="51" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="53"/>
+    <row r="2" spans="1:12" s="45" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="47"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="63" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
+      <c r="A3" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="57"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="57" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
+      <c r="K3" s="57"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="45" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="38" t="s">
+      <c r="A4" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="D4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="40" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="38" t="s">
+      <c r="G4" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="38" t="s">
+      <c r="J4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="46" t="s">
+      <c r="K4" s="40" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="56" t="s">
+      <c r="A5" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <f>'Spools by Scope'!B4</f>
         <v>0</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <f>'Spools by Scope'!C4</f>
         <v>0</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <f>'Spools by Scope'!D4</f>
         <v>0</v>
       </c>
-      <c r="E5" s="60">
+      <c r="E5" s="54">
         <f>SUM(B5:D5)</f>
         <v>0</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="56" t="s">
+      <c r="G5" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <f>'Purchased by Scope'!B4</f>
         <v>0</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <f>'Purchased by Scope'!C4</f>
         <v>0</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <f>'Purchased by Scope'!D4</f>
         <v>0</v>
       </c>
-      <c r="K5" s="60">
+      <c r="K5" s="54">
         <f>SUM(H5:J5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <f>'Spools by Scope'!B5</f>
         <v>0</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <f>'Spools by Scope'!C5</f>
         <v>0</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <f>'Spools by Scope'!D5</f>
         <v>0</v>
       </c>
-      <c r="E6" s="60">
+      <c r="E6" s="54">
         <f t="shared" ref="E6:E9" si="0">SUM(B6:D6)</f>
         <v>0</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="56" t="s">
+      <c r="G6" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <f>'Purchased by Scope'!B5</f>
         <v>0</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <f>'Purchased by Scope'!C5</f>
         <v>0</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <f>'Purchased by Scope'!D5</f>
         <v>0</v>
       </c>
-      <c r="K6" s="60">
+      <c r="K6" s="54">
         <f>SUM(H6:J6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
+      <c r="A7" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <f>'Spools by Scope'!B6</f>
         <v>0</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <f>'Spools by Scope'!C6</f>
         <v>0</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <f>'Spools by Scope'!D6</f>
         <v>0</v>
       </c>
-      <c r="E7" s="60">
+      <c r="E7" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="56" t="s">
+      <c r="G7" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <f>'Purchased by Scope'!B6</f>
         <v>0</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <f>'Purchased by Scope'!C6</f>
         <v>0</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <f>'Purchased by Scope'!D6</f>
         <v>0</v>
       </c>
-      <c r="K7" s="60">
+      <c r="K7" s="54">
         <f t="shared" ref="K7:K8" si="1">SUM(H7:J7)</f>
         <v>0</v>
       </c>
       <c r="L7"/>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <f>'Spools by Scope'!B7</f>
         <v>0</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <f>'Spools by Scope'!C7</f>
         <v>0</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <f>'Spools by Scope'!D7</f>
         <v>0</v>
       </c>
-      <c r="E8" s="60">
+      <c r="E8" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="56" t="s">
+      <c r="G8" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <f>'Purchased by Scope'!B7</f>
         <v>0</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <f>'Purchased by Scope'!C7</f>
         <v>0</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <f>'Purchased by Scope'!D7</f>
         <v>0</v>
       </c>
-      <c r="K8" s="60">
+      <c r="K8" s="54">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <f>'Spools by Scope'!B8</f>
         <v>0</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <f>'Spools by Scope'!C8</f>
         <v>0</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <f>'Spools by Scope'!D8</f>
         <v>0</v>
       </c>
-      <c r="E9" s="60">
+      <c r="E9" s="54">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="H9" s="43">
+      <c r="H9" s="37">
         <f>SUM(H5:H8)</f>
         <v>0</v>
       </c>
-      <c r="I9" s="43">
+      <c r="I9" s="37">
         <f>SUM(I5:I8)</f>
         <v>0</v>
       </c>
-      <c r="J9" s="43">
+      <c r="J9" s="37">
         <f>SUM(J5:J8)</f>
         <v>0</v>
       </c>
-      <c r="K9" s="44">
+      <c r="K9" s="38">
         <f t="shared" ref="K9" si="2">SUM(K5:K8)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="60">
+      <c r="A10" s="50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="54">
         <f>'Spools by Scope'!E9</f>
         <v>0</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="60">
+      <c r="A11" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="54">
         <f>'Spools by Scope'!E10</f>
         <v>0</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="57" t="s">
+      <c r="G11" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="H11" s="47">
+      <c r="H11" s="41">
         <f>'Purchased by Scope'!B10</f>
         <v>0</v>
       </c>
-      <c r="I11" s="47">
+      <c r="I11" s="41">
         <f>'Purchased by Scope'!C10</f>
         <v>0</v>
       </c>
-      <c r="J11" s="47">
+      <c r="J11" s="41">
         <f>'Purchased by Scope'!D10</f>
         <v>0</v>
       </c>
-      <c r="K11" s="48">
+      <c r="K11" s="42">
         <f>SUM(H11:J11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="60"/>
+      <c r="A12" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="54">
+        <f>'Spools by Scope'!E11</f>
+        <v>0</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -8959,13 +8871,16 @@
       <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="56" t="s">
-        <v>66</v>
-      </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="60"/>
+      <c r="A13" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="54">
+        <f>'Spools by Scope'!E12</f>
+        <v>0</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
@@ -8974,473 +8889,473 @@
       <c r="K13" s="2"/>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36"/>
-      <c r="E14" s="41">
-        <f>'Spools by Scope'!E11</f>
+      <c r="A14" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="35">
+        <f>'Spools by Scope'!E13</f>
         <v>0</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" s="63"/>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="63"/>
+      <c r="G14" s="57" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="57"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="57"/>
+      <c r="K14" s="57"/>
     </row>
-    <row r="15" spans="1:12" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="42" t="s">
+    <row r="15" spans="1:12" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="43">
+      <c r="B15" s="37">
         <f>SUM(B5:B9)</f>
         <v>0</v>
       </c>
-      <c r="C15" s="43">
+      <c r="C15" s="37">
         <f>SUM(C5:C9)</f>
         <v>0</v>
       </c>
-      <c r="D15" s="43">
+      <c r="D15" s="37">
         <f>SUM(D5:D9)</f>
         <v>0</v>
       </c>
-      <c r="E15" s="44">
-        <f>'Spools by Scope'!E12</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="H15" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="38" t="s">
+      <c r="E15" s="38">
+        <f>'Spools by Scope'!E14</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="I15" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="J15" s="38" t="s">
+      <c r="J15" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="K15" s="46" t="s">
+      <c r="K15" s="40" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G16" s="56" t="s">
+      <c r="G16" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <f>'No Material by Scope'!B4</f>
         <v>0</v>
       </c>
-      <c r="I16" s="6">
+      <c r="I16" s="5">
         <f>'No Material by Scope'!C4</f>
         <v>0</v>
       </c>
-      <c r="J16" s="6">
+      <c r="J16" s="5">
         <f>'No Material by Scope'!D4</f>
         <v>0</v>
       </c>
-      <c r="K16" s="60">
+      <c r="K16" s="54">
         <f>SUM(H16:J16)</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:14" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="63" t="s">
-        <v>49</v>
-      </c>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="56" t="s">
+      <c r="A17" s="57" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="57"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="57"/>
+      <c r="E17" s="57"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <f>'No Material by Scope'!B5</f>
         <v>0</v>
       </c>
-      <c r="I17" s="6">
+      <c r="I17" s="5">
         <f>'No Material by Scope'!C5</f>
         <v>0</v>
       </c>
-      <c r="J17" s="6">
+      <c r="J17" s="5">
         <f>'No Material by Scope'!D5</f>
         <v>0</v>
       </c>
-      <c r="K17" s="60">
+      <c r="K17" s="54">
         <f t="shared" ref="K17:K19" si="3">SUM(H17:J17)</f>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="B18" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="38" t="s">
+      <c r="A18" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="D18" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="E18" s="46" t="s">
+      <c r="E18" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="56" t="s">
+      <c r="F18" s="19"/>
+      <c r="G18" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="5">
         <f>'No Material by Scope'!B6</f>
         <v>0</v>
       </c>
-      <c r="I18" s="6">
+      <c r="I18" s="5">
         <f>'No Material by Scope'!C6</f>
         <v>0</v>
       </c>
-      <c r="J18" s="6">
+      <c r="J18" s="5">
         <f>'No Material by Scope'!D6</f>
         <v>0</v>
       </c>
-      <c r="K18" s="60">
+      <c r="K18" s="54">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <f>'Shorts by Scope'!B4</f>
         <v>0</v>
       </c>
-      <c r="C19" s="6">
+      <c r="C19" s="5">
         <f>'Shorts by Scope'!C4</f>
         <v>0</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="5">
         <f>'Shorts by Scope'!D4</f>
         <v>0</v>
       </c>
-      <c r="E19" s="60">
+      <c r="E19" s="54">
         <f>SUM(B19:D19)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="56" t="s">
+      <c r="F19" s="19"/>
+      <c r="G19" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="H19" s="6">
+      <c r="H19" s="5">
         <f>'No Material by Scope'!B7</f>
         <v>0</v>
       </c>
-      <c r="I19" s="6">
+      <c r="I19" s="5">
         <f>'No Material by Scope'!C7</f>
         <v>0</v>
       </c>
-      <c r="J19" s="6">
+      <c r="J19" s="5">
         <f>'No Material by Scope'!D7</f>
         <v>0</v>
       </c>
-      <c r="K19" s="60">
+      <c r="K19" s="54">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="6">
+      <c r="B20" s="5">
         <f>'Shorts by Scope'!B5</f>
         <v>0</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="5">
         <f>'Shorts by Scope'!C5</f>
         <v>0</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="5">
         <f>'Shorts by Scope'!D5</f>
         <v>0</v>
       </c>
-      <c r="E20" s="60">
+      <c r="E20" s="54">
         <f t="shared" ref="E20:E22" si="4">SUM(B20:D20)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="42" t="s">
+      <c r="F20" s="19"/>
+      <c r="G20" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="H20" s="43">
+      <c r="H20" s="37">
         <f>SUM(H16:H19)</f>
         <v>0</v>
       </c>
-      <c r="I20" s="43">
+      <c r="I20" s="37">
         <f t="shared" ref="I20:K20" si="5">SUM(I16:I19)</f>
         <v>0</v>
       </c>
-      <c r="J20" s="43">
+      <c r="J20" s="37">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K20" s="44">
+      <c r="K20" s="38">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="5">
         <f>'Shorts by Scope'!B6</f>
         <v>0</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="5">
         <f>'Shorts by Scope'!C6</f>
         <v>0</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="5">
         <f>'Shorts by Scope'!D6</f>
         <v>0</v>
       </c>
-      <c r="E21" s="60">
+      <c r="E21" s="54">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F21" s="21"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="B22" s="6">
+      <c r="B22" s="5">
         <f>'Shorts by Scope'!B7</f>
         <v>0</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="5">
         <f>'Shorts by Scope'!C7</f>
         <v>0</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="5">
         <f>'Shorts by Scope'!D7</f>
         <v>0</v>
       </c>
-      <c r="E22" s="60">
+      <c r="E22" s="54">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F22" s="21"/>
-      <c r="G22" s="57" t="s">
+      <c r="F22" s="19"/>
+      <c r="G22" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="H22" s="47">
+      <c r="H22" s="41">
         <f>'No Material by Scope'!B10</f>
         <v>0</v>
       </c>
-      <c r="I22" s="47">
+      <c r="I22" s="41">
         <f>'No Material by Scope'!C10</f>
         <v>0</v>
       </c>
-      <c r="J22" s="47">
+      <c r="J22" s="41">
         <f>'No Material by Scope'!D10</f>
         <v>0</v>
       </c>
-      <c r="K22" s="48">
+      <c r="K22" s="42">
         <f>SUM(H22:J22)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="17" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="42" t="s">
+    <row r="23" spans="1:14" s="15" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="43">
+      <c r="B23" s="37">
         <f>SUM(B19:B22)</f>
         <v>0</v>
       </c>
-      <c r="C23" s="43">
+      <c r="C23" s="37">
         <f t="shared" ref="C23:E23" si="6">SUM(C19:C22)</f>
         <v>0</v>
       </c>
-      <c r="D23" s="43">
+      <c r="D23" s="37">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E23" s="44">
+      <c r="E23" s="38">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F23" s="22"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="23"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="33"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:14" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="47">
+      <c r="B25" s="41">
         <f>'Shorts by Scope'!B10</f>
         <v>0</v>
       </c>
-      <c r="C25" s="47">
+      <c r="C25" s="41">
         <f>'Shorts by Scope'!C10</f>
         <v>0</v>
       </c>
-      <c r="D25" s="47">
+      <c r="D25" s="41">
         <f>'Shorts by Scope'!D10</f>
         <v>0</v>
       </c>
-      <c r="E25" s="48">
+      <c r="E25" s="42">
         <f>SUM(B25:D25)</f>
         <v>0</v>
       </c>
-      <c r="F25" s="23"/>
-      <c r="G25" s="63" t="s">
-        <v>52</v>
-      </c>
-      <c r="H25" s="63"/>
-      <c r="I25" s="63"/>
-      <c r="J25" s="63"/>
-      <c r="K25" s="63"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="57"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="57"/>
+      <c r="K25" s="57"/>
     </row>
     <row r="26" spans="1:14" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="45" t="s">
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="I26" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J26" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="K26" s="40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="H26" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="J26" s="38" t="s">
-        <v>2</v>
-      </c>
-      <c r="K26" s="46" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" s="21" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="34">
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="28">
         <f>'Shorts by Scope'!E12</f>
         <v>0</v>
       </c>
-      <c r="F27" s="37"/>
-      <c r="G27" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" s="49">
+      <c r="F27" s="31"/>
+      <c r="G27" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="43">
         <f>'Spool Missing Valve Only'!B3</f>
         <v>0</v>
       </c>
-      <c r="I27" s="49">
+      <c r="I27" s="43">
         <f>'Spool Missing Valve Only'!C3</f>
         <v>0</v>
       </c>
-      <c r="J27" s="49">
+      <c r="J27" s="43">
         <f>'Spool Missing Valve Only'!D3</f>
         <v>0</v>
       </c>
-      <c r="K27" s="50">
+      <c r="K27" s="44">
         <f>SUM(H27:J27)</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="64"/>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="64"/>
-      <c r="J31" s="64"/>
-      <c r="K31" s="64"/>
-      <c r="L31" s="64"/>
-      <c r="M31" s="64"/>
-      <c r="N31" s="64"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="58"/>
+      <c r="I31" s="58"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="58"/>
+      <c r="L31" s="58"/>
+      <c r="M31" s="58"/>
+      <c r="N31" s="58"/>
     </row>
     <row r="32" spans="1:14" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="59" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="59" t="s">
+      <c r="A32" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="53" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="53" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="53" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="C32" s="59" t="s">
-        <v>55</v>
-      </c>
-      <c r="D32" s="59" t="s">
-        <v>64</v>
-      </c>
-      <c r="E32" s="59" t="s">
+      <c r="I32" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="J32" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="F32" s="59" t="s">
-        <v>42</v>
-      </c>
-      <c r="G32" s="59" t="s">
+      <c r="K32" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="H32" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="I32" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="J32" s="59" t="s">
+      <c r="L32" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="M32" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="K32" s="59" t="s">
-        <v>58</v>
-      </c>
-      <c r="L32" s="59" t="s">
-        <v>59</v>
-      </c>
-      <c r="M32" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="N32" s="59" t="s">
-        <v>61</v>
+      <c r="N32" s="53" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -9449,69 +9364,6 @@
     <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A31:N31"/>
@@ -9532,445 +9384,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:H1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15" style="31" customWidth="1"/>
-    <col min="2" max="2" width="20" style="31" customWidth="1"/>
-    <col min="3" max="3" width="30" style="31" customWidth="1"/>
-    <col min="4" max="4" width="20" style="31" customWidth="1"/>
-    <col min="5" max="5" width="28" style="31" customWidth="1"/>
-    <col min="6" max="7" width="21" style="31" customWidth="1"/>
-    <col min="8" max="8" width="13.85546875" style="31" customWidth="1"/>
-    <col min="9" max="11" width="9.7109375" style="31" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="31"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" s="30" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{FB8E7C81-D36E-456C-ABC3-21D3748C3168}"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:K13"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="5" width="24" style="1" customWidth="1"/>
-    <col min="6" max="8" width="9.140625" style="1"/>
-    <col min="9" max="9" width="43" style="1" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="43" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="4">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4">
-        <f>F2</f>
-        <v>0</v>
-      </c>
-      <c r="D1" s="4">
-        <f>F4</f>
-        <v>0</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="21"/>
-    </row>
-    <row r="2" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
-        <v>28</v>
-      </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="21"/>
-    </row>
-    <row r="3" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="24">
-        <f>SUM(B4:D4)</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="24">
-        <f t="shared" ref="E5:E10" si="0">SUM(B5:D5)</f>
-        <v>0</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="34">
-        <f>ABS(E12-SUM(E4:E10))</f>
-        <v>0</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="20">
-        <f>SUM(B4:B8)</f>
-        <v>0</v>
-      </c>
-      <c r="C12" s="20">
-        <f t="shared" ref="C12:D12" si="1">SUM(C4:C8)</f>
-        <v>0</v>
-      </c>
-      <c r="D12" s="20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="26"/>
-      <c r="F12" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-    </row>
-    <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:E2"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35C9E26B-5273-455B-9FB2-6884F9EF8210}">
-  <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Z1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="18.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.7109375" style="15" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="16.7109375" style="3" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="3" customWidth="1"/>
-    <col min="12" max="12" width="17" style="3" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="24.85546875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="16.7109375" style="3" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="19" style="3" customWidth="1"/>
-    <col min="20" max="20" width="24.140625" style="3" customWidth="1"/>
-    <col min="21" max="23" width="21.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="22.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="16.28515625" style="3" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" style="3" customWidth="1"/>
-    <col min="27" max="16384" width="18.28515625" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" s="28" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J1" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" s="27" t="s">
-        <v>38</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="T1" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="U1" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="V1" s="27" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="27" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z1" s="27" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:Z1" xr:uid="{6B087137-8043-4B5F-87A7-6CEB5CAC1499}"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B72B38F-98DC-4DB7-A570-DD1AB8DD070C}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:D1"/>
@@ -9986,18 +9399,18 @@
     <col min="5" max="16384" width="12.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="16" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>63</v>
+    <row r="1" spans="1:4" s="14" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -10007,19 +9420,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42879D7-E02D-48D6-B3BF-3D5D974FF711}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1E0543F-5887-4AAB-B5E8-E7459CA2FA09}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -10031,7 +9431,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51053A3-1560-45FC-B69A-E4BBE7985B1A}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -10045,7 +9445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{201222A3-BE08-4C87-870E-382DD255A082}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B9"/>
@@ -10056,58 +9456,58 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="14"/>
+    <col min="1" max="2" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="32"/>
+      <c r="A1" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="26"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="32"/>
+      <c r="A2" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="26"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="32" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="32"/>
+      <c r="A3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="26"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="32"/>
+      <c r="A4" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="26"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B5" s="32"/>
+      <c r="A5" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="26"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B6" s="32"/>
+      <c r="A6" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="26"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="32"/>
+      <c r="A7" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="26"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="26"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="32"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10115,181 +9515,181 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="24.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="21"/>
+    <col min="6" max="6" width="9.140625" style="19"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="4">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4">
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
         <f>F2</f>
         <v>0</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <f>F4</f>
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
+      <c r="A2" s="59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="3" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="18">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="16">
         <f>SUM(B4:D4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="18">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="16">
         <f t="shared" ref="E5:E7" si="0">SUM(B5:D5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="18">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="18">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="17" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:11" s="15" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="18">
         <f>SUM(B4:B7)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="18">
         <f t="shared" ref="C8:E8" si="1">SUM(C4:C7)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="22"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="23"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:11" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12">
         <f>SUM(B10:D10)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="23"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="21"/>
     </row>
-    <row r="12" spans="1:11" s="21" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36"/>
-      <c r="D12" s="36"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="37"/>
-      <c r="K12" s="37"/>
+    <row r="12" spans="1:11" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
     </row>
     <row r="13" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F13" s="23"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="23"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
@@ -10307,7 +9707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F84688-247E-4A82-AFB3-DC27342D02F1}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -10318,146 +9718,146 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="24.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="21"/>
+    <col min="6" max="6" width="9.140625" style="19"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="4">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4">
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
         <f>F2</f>
         <v>0</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <f>F4</f>
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
+      <c r="A2" s="59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="18">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="16">
         <f>SUM(B4:D4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="18">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="16">
         <f>SUM(B5:D5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="18">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="16">
         <f t="shared" ref="E6:E7" si="0">SUM(B6:D6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="18">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="17" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:6" s="15" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="18">
         <f>SUM(B4:B7)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="18">
         <f>SUM(C4:C7)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="18">
         <f>SUM(D4:D7)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="18">
         <f t="shared" ref="E8" si="1">SUM(E4:E7)</f>
         <v>0</v>
       </c>
-      <c r="F8" s="22"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="23"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="13">
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="12">
         <f>SUM(B10:D10)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="23"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="23"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -10476,7 +9876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C47B9C1C-94EB-4EC1-82B7-F8B9C143A6F1}">
   <dimension ref="A1:F13"/>
   <sheetViews>
@@ -10487,146 +9887,146 @@
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="24.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="21"/>
+    <col min="6" max="6" width="9.140625" style="19"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="4">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4">
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
         <f>F2</f>
         <v>0</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="3">
         <f>F4</f>
         <v>0</v>
       </c>
-      <c r="E1" s="4"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
+      <c r="A2" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="59"/>
+      <c r="C2" s="59"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="59"/>
     </row>
     <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="18">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="16">
         <f>SUM(B4:D4)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="18">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="16">
         <f t="shared" ref="E5:E7" si="0">SUM(B5:D5)</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="18">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="18">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="17" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:6" s="15" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="18">
         <f>SUM(B4:B7)</f>
         <v>0</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="18">
         <f t="shared" ref="C8:E8" si="1">SUM(C4:C7)</f>
         <v>0</v>
       </c>
-      <c r="D8" s="20">
+      <c r="D8" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F8" s="22"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="23"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="13">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="12">
         <f>SUM(B10:D10)</f>
         <v>0</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F11" s="23"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F12" s="23"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
@@ -10644,7 +10044,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B523AC-4D5C-44BB-920E-D987B5985E0A}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -10659,39 +10059,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
+      <c r="A1" s="59" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="9" t="s">
+      <c r="A2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="18">
+      <c r="A3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="16">
         <f>SUM(B3:D3)</f>
         <v>0</v>
       </c>
@@ -10702,6 +10102,287 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Sheet4"/>
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="24" style="1" customWidth="1"/>
+    <col min="6" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="43" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="43" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="3">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3">
+        <f>F2</f>
+        <v>0</v>
+      </c>
+      <c r="D1" s="3">
+        <f>F4</f>
+        <v>0</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="60" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="22">
+        <f>SUM(B4:D4)</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="22">
+        <f t="shared" ref="E5:E8" si="0">SUM(B5:D5)</f>
+        <v>0</v>
+      </c>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="22"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="18">
+        <f>SUM(B4:B8)</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="18">
+        <f t="shared" ref="C14:D14" si="1">SUM(C4:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="24"/>
+      <c r="F14" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add man hours to job summary
</commit_message>
<xml_diff>
--- a/database/Templates/JobSumTemplate.xlsx
+++ b/database/Templates/JobSumTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kurtm\Documents\GitHub\PerformanceHub\database\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{49C11806-7A00-4585-B19C-CF9990090FD3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6FB9CBFC-F867-4D80-B230-B79C473DD28B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8685" tabRatio="820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="50">
   <si>
     <t>Performance</t>
   </si>
@@ -168,12 +168,24 @@
   <si>
     <t>Ready To Deliver</t>
   </si>
+  <si>
+    <t>Workable Man Hours (By Material)</t>
+  </si>
+  <si>
+    <t>Carbon</t>
+  </si>
+  <si>
+    <t>Stainless</t>
+  </si>
+  <si>
+    <t>Workable Man Hours</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,12 +287,14 @@
       <sz val="20"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -293,6 +307,13 @@
     <font>
       <b/>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -638,7 +659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -771,18 +792,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -798,23 +807,62 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8512,65 +8560,66 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="5" width="16.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="11" width="21.42578125" customWidth="1"/>
-    <col min="12" max="13" width="14.42578125" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" style="69" customWidth="1"/>
+    <col min="2" max="5" width="16.5703125" style="69" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="69" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" style="69" customWidth="1"/>
+    <col min="8" max="11" width="21.42578125" style="69" customWidth="1"/>
+    <col min="12" max="13" width="14.42578125" style="69" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" style="69" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="69"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="46" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="57"/>
-      <c r="B1" s="57"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="49"/>
+    <row r="1" spans="1:12" s="45" customFormat="1" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="59"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="63"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
     </row>
     <row r="2" spans="1:12" s="45" customFormat="1" ht="13.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="47"/>
-      <c r="B2" s="47"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="47"/>
+      <c r="A2" s="67"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="67"/>
     </row>
     <row r="3" spans="1:12" s="1" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="56"/>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
       <c r="F3" s="19"/>
-      <c r="G3" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-      <c r="K3" s="56"/>
+      <c r="G3" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
     </row>
     <row r="4" spans="1:12" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
@@ -8589,24 +8638,20 @@
         <v>3</v>
       </c>
       <c r="F4" s="2"/>
-      <c r="G4" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="32" t="s">
-        <v>0</v>
-      </c>
+      <c r="G4" s="55"/>
+      <c r="H4" s="56"/>
       <c r="I4" s="32" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="J4" s="32" t="s">
-        <v>2</v>
+        <v>48</v>
       </c>
       <c r="K4" s="40" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="46" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="5">
@@ -8621,33 +8666,21 @@
         <f>'Spools by Scope'!D4</f>
         <v>0</v>
       </c>
-      <c r="E5" s="54">
+      <c r="E5" s="50">
         <f>SUM(B5:D5)</f>
         <v>0</v>
       </c>
       <c r="F5" s="2"/>
-      <c r="G5" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="5">
-        <f>'Purchased by Scope'!B4</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <f>'Purchased by Scope'!C4</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
-        <f>'Purchased by Scope'!D4</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="54">
-        <f>SUM(H5:J5)</f>
-        <v>0</v>
-      </c>
+      <c r="G5" s="57" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="58"/>
+      <c r="I5" s="43"/>
+      <c r="J5" s="43"/>
+      <c r="K5" s="44"/>
     </row>
     <row r="6" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="50" t="s">
+      <c r="A6" s="46" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5">
@@ -8662,33 +8695,14 @@
         <f>'Spools by Scope'!D5</f>
         <v>0</v>
       </c>
-      <c r="E6" s="54">
+      <c r="E6" s="50">
         <f t="shared" ref="E6:E9" si="0">SUM(B6:D6)</f>
         <v>0</v>
       </c>
       <c r="F6" s="2"/>
-      <c r="G6" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="5">
-        <f>'Purchased by Scope'!B5</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <f>'Purchased by Scope'!C5</f>
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
-        <f>'Purchased by Scope'!D5</f>
-        <v>0</v>
-      </c>
-      <c r="K6" s="54">
-        <f>SUM(H6:J6)</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="50" t="s">
+      <c r="A7" s="46" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="5">
@@ -8703,34 +8717,22 @@
         <f>'Spools by Scope'!D6</f>
         <v>0</v>
       </c>
-      <c r="E7" s="54">
+      <c r="E7" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F7" s="2"/>
-      <c r="G7" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="H7" s="5">
-        <f>'Purchased by Scope'!B6</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <f>'Purchased by Scope'!C6</f>
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <f>'Purchased by Scope'!D6</f>
-        <v>0</v>
-      </c>
-      <c r="K7" s="54">
-        <f t="shared" ref="K7:K8" si="1">SUM(H7:J7)</f>
-        <v>0</v>
-      </c>
-      <c r="L7"/>
+      <c r="G7" s="51" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="51"/>
+      <c r="I7" s="51"/>
+      <c r="J7" s="51"/>
+      <c r="K7" s="51"/>
+      <c r="L7" s="69"/>
     </row>
     <row r="8" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="50" t="s">
+      <c r="A8" s="46" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="5">
@@ -8745,33 +8747,29 @@
         <f>'Spools by Scope'!D7</f>
         <v>0</v>
       </c>
-      <c r="E8" s="54">
+      <c r="E8" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F8" s="2"/>
-      <c r="G8" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="5">
-        <f>'Purchased by Scope'!B7</f>
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
-        <f>'Purchased by Scope'!C7</f>
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
-        <f>'Purchased by Scope'!D7</f>
-        <v>0</v>
-      </c>
-      <c r="K8" s="54">
-        <f t="shared" si="1"/>
-        <v>0</v>
+      <c r="G8" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="I8" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="40" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="50" t="s">
+      <c r="A9" s="46" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="5">
@@ -8786,116 +8784,158 @@
         <f>'Spools by Scope'!D8</f>
         <v>0</v>
       </c>
-      <c r="E9" s="54">
+      <c r="E9" s="50">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="37">
-        <f>SUM(H5:H8)</f>
-        <v>0</v>
-      </c>
-      <c r="I9" s="37">
-        <f>SUM(I5:I8)</f>
-        <v>0</v>
-      </c>
-      <c r="J9" s="37">
-        <f>SUM(J5:J8)</f>
-        <v>0</v>
-      </c>
-      <c r="K9" s="38">
-        <f t="shared" ref="K9" si="2">SUM(K5:K8)</f>
+      <c r="G9" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="5">
+        <f>'Purchased by Scope'!B4</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <f>'Purchased by Scope'!C4</f>
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <f>'Purchased by Scope'!D4</f>
+        <v>0</v>
+      </c>
+      <c r="K9" s="50">
+        <f>SUM(H9:J9)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="50" t="s">
+      <c r="A10" s="46" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
-      <c r="E10" s="54">
+      <c r="E10" s="50">
         <f>'Spools by Scope'!E9</f>
         <v>0</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="G10" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10" s="5">
+        <f>'Purchased by Scope'!B5</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <f>'Purchased by Scope'!C5</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <f>'Purchased by Scope'!D5</f>
+        <v>0</v>
+      </c>
+      <c r="K10" s="50">
+        <f>SUM(H10:J10)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="46" t="s">
         <v>43</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
-      <c r="E11" s="54">
+      <c r="E11" s="50">
         <f>'Spools by Scope'!E10</f>
         <v>0</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="H11" s="41">
-        <f>'Purchased by Scope'!B10</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="41">
-        <f>'Purchased by Scope'!C10</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="41">
-        <f>'Purchased by Scope'!D10</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="42">
-        <f>SUM(H11:J11)</f>
+      <c r="G11" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11" s="5">
+        <f>'Purchased by Scope'!B6</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <f>'Purchased by Scope'!C6</f>
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <f>'Purchased by Scope'!D6</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="50">
+        <f t="shared" ref="K11:K12" si="1">SUM(H11:J11)</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="50" t="s">
+      <c r="A12" s="46" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="54">
+      <c r="E12" s="50">
         <f>'Spools by Scope'!E11</f>
         <v>0</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
+      <c r="G12" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="5">
+        <f>'Purchased by Scope'!B7</f>
+        <v>0</v>
+      </c>
+      <c r="I12" s="5">
+        <f>'Purchased by Scope'!C7</f>
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <f>'Purchased by Scope'!D7</f>
+        <v>0</v>
+      </c>
+      <c r="K12" s="50">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="46" t="s">
         <v>44</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="54">
+      <c r="E13" s="50">
         <f>'Spools by Scope'!E12</f>
         <v>0</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
+      <c r="G13" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="37">
+        <f>SUM(H9:H12)</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="37">
+        <f>SUM(I9:I12)</f>
+        <v>0</v>
+      </c>
+      <c r="J13" s="37">
+        <f>SUM(J9:J12)</f>
+        <v>0</v>
+      </c>
+      <c r="K13" s="38">
+        <f t="shared" ref="K13" si="2">SUM(K9:K12)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:12" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="34" t="s">
@@ -8909,13 +8949,11 @@
         <v>0</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="56" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:12" s="15" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36" t="s">
@@ -8940,71 +8978,49 @@
       <c r="F15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="I15" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="40" t="s">
-        <v>3</v>
+      <c r="G15" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="41">
+        <f>'Purchased by Scope'!B10</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="41">
+        <f>'Purchased by Scope'!C10</f>
+        <v>0</v>
+      </c>
+      <c r="J15" s="41">
+        <f>'Purchased by Scope'!D10</f>
+        <v>0</v>
+      </c>
+      <c r="K15" s="42">
+        <f>SUM(H15:J15)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G16" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="H16" s="5">
-        <f>'No Material by Scope'!B4</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="5">
-        <f>'No Material by Scope'!C4</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="5">
-        <f>'No Material by Scope'!D4</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="54">
-        <f>SUM(H16:J16)</f>
-        <v>0</v>
-      </c>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="51"/>
     </row>
     <row r="17" spans="1:14" s="1" customFormat="1" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="51" t="s">
         <v>28</v>
       </c>
-      <c r="B17" s="56"/>
-      <c r="C17" s="56"/>
-      <c r="D17" s="56"/>
-      <c r="E17" s="56"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="51"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="19"/>
-      <c r="G17" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="H17" s="5">
-        <f>'No Material by Scope'!B5</f>
-        <v>0</v>
-      </c>
-      <c r="I17" s="5">
-        <f>'No Material by Scope'!C5</f>
-        <v>0</v>
-      </c>
-      <c r="J17" s="5">
-        <f>'No Material by Scope'!D5</f>
-        <v>0</v>
-      </c>
-      <c r="K17" s="54">
-        <f t="shared" ref="K17:K19" si="3">SUM(H17:J17)</f>
-        <v>0</v>
-      </c>
+      <c r="G17" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
+      <c r="K17" s="51"/>
     </row>
     <row r="18" spans="1:14" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="39" t="s">
@@ -9023,28 +9039,24 @@
         <v>3</v>
       </c>
       <c r="F18" s="19"/>
-      <c r="G18" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="H18" s="5">
-        <f>'No Material by Scope'!B6</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="5">
-        <f>'No Material by Scope'!C6</f>
-        <v>0</v>
-      </c>
-      <c r="J18" s="5">
-        <f>'No Material by Scope'!D6</f>
-        <v>0</v>
-      </c>
-      <c r="K18" s="54">
-        <f t="shared" si="3"/>
-        <v>0</v>
+      <c r="G18" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="I18" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="K18" s="40" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="50" t="s">
+      <c r="A19" s="46" t="s">
         <v>4</v>
       </c>
       <c r="B19" s="5">
@@ -9059,33 +9071,33 @@
         <f>'Shorts by Scope'!D4</f>
         <v>0</v>
       </c>
-      <c r="E19" s="54">
+      <c r="E19" s="50">
         <f>SUM(B19:D19)</f>
         <v>0</v>
       </c>
       <c r="F19" s="19"/>
-      <c r="G19" s="50" t="s">
-        <v>8</v>
+      <c r="G19" s="46" t="s">
+        <v>4</v>
       </c>
       <c r="H19" s="5">
-        <f>'No Material by Scope'!B7</f>
+        <f>'No Material by Scope'!B5</f>
         <v>0</v>
       </c>
       <c r="I19" s="5">
-        <f>'No Material by Scope'!C7</f>
+        <f>'No Material by Scope'!C5</f>
         <v>0</v>
       </c>
       <c r="J19" s="5">
-        <f>'No Material by Scope'!D7</f>
-        <v>0</v>
-      </c>
-      <c r="K19" s="54">
-        <f t="shared" si="3"/>
+        <f>'No Material by Scope'!D5</f>
+        <v>0</v>
+      </c>
+      <c r="K19" s="50">
+        <f>SUM(H19:J19)</f>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="50" t="s">
+      <c r="A20" s="46" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="5">
@@ -9100,33 +9112,33 @@
         <f>'Shorts by Scope'!D5</f>
         <v>0</v>
       </c>
-      <c r="E20" s="54">
-        <f t="shared" ref="E20:E22" si="4">SUM(B20:D20)</f>
+      <c r="E20" s="50">
+        <f t="shared" ref="E20:E22" si="3">SUM(B20:D20)</f>
         <v>0</v>
       </c>
       <c r="F20" s="19"/>
-      <c r="G20" s="36" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" s="37">
-        <f>SUM(H16:H19)</f>
-        <v>0</v>
-      </c>
-      <c r="I20" s="37">
-        <f t="shared" ref="I20:K20" si="5">SUM(I16:I19)</f>
-        <v>0</v>
-      </c>
-      <c r="J20" s="37">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K20" s="38">
-        <f t="shared" si="5"/>
+      <c r="G20" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="5">
+        <f>'No Material by Scope'!B6</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="5">
+        <f>'No Material by Scope'!C6</f>
+        <v>0</v>
+      </c>
+      <c r="J20" s="5">
+        <f>'No Material by Scope'!D6</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="50">
+        <f t="shared" ref="K20:K24" si="4">SUM(H20:J20)</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="50" t="s">
+      <c r="A21" s="46" t="s">
         <v>6</v>
       </c>
       <c r="B21" s="5">
@@ -9141,19 +9153,33 @@
         <f>'Shorts by Scope'!D6</f>
         <v>0</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="46" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" s="5">
+        <f>'No Material by Scope'!B7</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="5">
+        <f>'No Material by Scope'!C7</f>
+        <v>0</v>
+      </c>
+      <c r="J21" s="5">
+        <f>'No Material by Scope'!D7</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="50">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:14" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="50" t="s">
+      <c r="A22" s="46" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="5">
@@ -9168,28 +9194,28 @@
         <f>'Shorts by Scope'!D7</f>
         <v>0</v>
       </c>
-      <c r="E22" s="54">
+      <c r="E22" s="50">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="5">
+        <f>'No Material by Scope'!B8</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="5">
+        <f>'No Material by Scope'!C8</f>
+        <v>0</v>
+      </c>
+      <c r="J22" s="5">
+        <f>'No Material by Scope'!D8</f>
+        <v>0</v>
+      </c>
+      <c r="K22" s="50">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="41">
-        <f>'No Material by Scope'!B10</f>
-        <v>0</v>
-      </c>
-      <c r="I22" s="41">
-        <f>'No Material by Scope'!C10</f>
-        <v>0</v>
-      </c>
-      <c r="J22" s="41">
-        <f>'No Material by Scope'!D10</f>
-        <v>0</v>
-      </c>
-      <c r="K22" s="42">
-        <f>SUM(H22:J22)</f>
         <v>0</v>
       </c>
     </row>
@@ -9202,18 +9228,37 @@
         <v>0</v>
       </c>
       <c r="C23" s="37">
-        <f t="shared" ref="C23:E23" si="6">SUM(C19:C22)</f>
+        <f t="shared" ref="C23:E23" si="5">SUM(C19:C22)</f>
         <v>0</v>
       </c>
       <c r="D23" s="37">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="F23" s="20"/>
+      <c r="G23" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="37">
+        <f>SUM(H19:H22)</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="37">
+        <f t="shared" ref="I23:K23" si="6">SUM(I19:I22)</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="37">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="E23" s="38">
+      <c r="K23" s="38">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:14" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
@@ -9222,9 +9267,14 @@
       <c r="D24" s="33"/>
       <c r="E24" s="4"/>
       <c r="F24" s="21"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:14" s="1" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="51" t="s">
+      <c r="A25" s="47" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="41">
@@ -9244,13 +9294,25 @@
         <v>0</v>
       </c>
       <c r="F25" s="21"/>
-      <c r="G25" s="56" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="56"/>
-      <c r="I25" s="56"/>
-      <c r="J25" s="56"/>
-      <c r="K25" s="56"/>
+      <c r="G25" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="41">
+        <f>'No Material by Scope'!B11</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="41">
+        <f>'No Material by Scope'!C11</f>
+        <v>0</v>
+      </c>
+      <c r="J25" s="41">
+        <f>'No Material by Scope'!D11</f>
+        <v>0</v>
+      </c>
+      <c r="K25" s="42">
+        <f>SUM(H25:J25)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:14" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
@@ -9259,21 +9321,11 @@
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="21"/>
-      <c r="G26" s="39" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="I26" s="32" t="s">
-        <v>1</v>
-      </c>
-      <c r="J26" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="K26" s="40" t="s">
-        <v>3</v>
-      </c>
+      <c r="G26" s="51"/>
+      <c r="H26" s="51"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="51"/>
+      <c r="K26" s="51"/>
     </row>
     <row r="27" spans="1:14" s="19" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
@@ -9287,104 +9339,131 @@
         <v>0</v>
       </c>
       <c r="F27" s="31"/>
-      <c r="G27" s="52" t="s">
+      <c r="G27" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="51"/>
+      <c r="I27" s="51"/>
+      <c r="J27" s="51"/>
+      <c r="K27" s="51"/>
+    </row>
+    <row r="28" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="G28" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="K28" s="40" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G29" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="H27" s="43">
-        <f>'Spool Missing Valve Only'!B3</f>
-        <v>0</v>
-      </c>
-      <c r="I27" s="43">
-        <f>'Spool Missing Valve Only'!C3</f>
-        <v>0</v>
-      </c>
-      <c r="J27" s="43">
-        <f>'Spool Missing Valve Only'!D3</f>
-        <v>0</v>
-      </c>
-      <c r="K27" s="44">
-        <f>SUM(H27:J27)</f>
+      <c r="H29" s="43">
+        <f>'Spool Missing Valve Only'!B4</f>
+        <v>0</v>
+      </c>
+      <c r="I29" s="43">
+        <f>'Spool Missing Valve Only'!C4</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="43">
+        <f>'Spool Missing Valve Only'!D4</f>
+        <v>0</v>
+      </c>
+      <c r="K29" s="44">
+        <f>SUM(H29:J29)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="55"/>
-      <c r="F31" s="55"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="55"/>
-      <c r="I31" s="55"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="55"/>
-      <c r="M31" s="55"/>
-      <c r="N31" s="55"/>
+    <row r="32" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="52"/>
+      <c r="B32" s="52"/>
+      <c r="C32" s="52"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="52"/>
+      <c r="N32" s="52"/>
     </row>
-    <row r="32" spans="1:14" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="53" t="s">
+    <row r="33" spans="1:14" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="53" t="s">
+      <c r="B33" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="53" t="s">
+      <c r="C33" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="53" t="s">
+      <c r="D33" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="53" t="s">
+      <c r="E33" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="F32" s="53" t="s">
+      <c r="F33" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="53" t="s">
+      <c r="G33" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="H32" s="53" t="s">
+      <c r="H33" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="I32" s="53" t="s">
+      <c r="I33" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="J32" s="53" t="s">
+      <c r="J33" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="K32" s="53" t="s">
+      <c r="K33" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="L32" s="53" t="s">
+      <c r="L33" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="M32" s="53" t="s">
+      <c r="M33" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="N32" s="53" t="s">
+      <c r="N33" s="49" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="I1:J1"/>
+  <mergeCells count="11">
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A31:N31"/>
-    <mergeCell ref="G14:K14"/>
+    <mergeCell ref="A32:N32"/>
     <mergeCell ref="A17:E17"/>
+    <mergeCell ref="G7:K7"/>
+    <mergeCell ref="G16:K16"/>
+    <mergeCell ref="G26:K26"/>
     <mergeCell ref="G3:K3"/>
-    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="G17:K17"/>
+    <mergeCell ref="G27:K27"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="G5:H5"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.3" footer="0.3"/>
   <pageSetup paperSize="17" scale="88" fitToHeight="0" orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -9559,13 +9638,13 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="3" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -9750,13 +9829,13 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -9919,13 +9998,13 @@
       <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
     </row>
     <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -10072,13 +10151,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -10153,13 +10232,13 @@
       <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="60"/>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
       <c r="F2" s="19"/>
     </row>
     <row r="3" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>